<commit_message>
update MULTI_RES occupant density
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/CH_ReMaP/archetypes/URB_2040_DGT/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/remap_ville_plugin/CH_ReMaP/archetypes/URB_2040_DGT/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shsieh\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\URB_2040_DGT\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B629481-88A8-4305-A4FF-6112297DC108}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319AE3EC-2E4F-437C-B9FB-525A0A7B7782}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15225" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTERNAL_LOADS" sheetId="1" r:id="rId1"/>
@@ -551,7 +551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -622,7 +622,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="9">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C2" s="9">
         <v>70</v>
@@ -1517,7 +1517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>